<commit_message>
exported GC summary excel sheets now have standard curve graphs inserted
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-Rprocessed/GC-Runs-Summary-Info/GCRunSummary_20131104_AA.xlsx
+++ b/GC-Data-Raw-R/GC-Data-Rprocessed/GC-Runs-Summary-Info/GCRunSummary_20131104_AA.xlsx
@@ -6,8 +6,11 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="GC Run Summary Info" r:id="rId3" sheetId="1"/>
+    <sheet name="GCRunSummaryInfo" r:id="rId3" sheetId="1"/>
   </sheets>
+  <definedNames>
+    <definedName name="graphs">GCRunSummaryInfo!$H$5</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -377,8 +380,51 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>19055</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="4286250" cy="8572500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
@@ -1518,5 +1564,6 @@
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>